<commit_message>
More on Sankey diagram
</commit_message>
<xml_diff>
--- a/chapters/ch09-Agriculture/datasets/Ag Sankey.xlsx
+++ b/chapters/ch09-Agriculture/datasets/Ag Sankey.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63338B8-1045-6843-A731-45DD0D2D0AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D7A4034-529A-C64C-9EE1-C74D8F51D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="17440" xr2:uid="{AC192F2F-F1F4-CC41-936B-E23658F68C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>x</t>
   </si>
@@ -79,6 +80,33 @@
   </si>
   <si>
     <t>Cultivated fields</t>
+  </si>
+  <si>
+    <t>Feed grains</t>
+  </si>
+  <si>
+    <t>Exports</t>
+  </si>
+  <si>
+    <t>Wheat &amp; flour</t>
+  </si>
+  <si>
+    <t>Oil seeds</t>
+  </si>
+  <si>
+    <t>Feeds &amp; fodders</t>
+  </si>
+  <si>
+    <t>Protein meal</t>
+  </si>
+  <si>
+    <t>Fruits, nuts &amp; preparations</t>
+  </si>
+  <si>
+    <t>Rice</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -479,15 +507,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCFF141-0596-C145-89EB-7AFC488BD6D2}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12:E15"/>
+      <selection activeCell="A17" sqref="A17:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="7.33203125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -747,8 +778,175 @@
         <v>611340</v>
       </c>
     </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>355560</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17">
+        <v>147260</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18">
+        <v>73620</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19">
+        <v>52020</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20">
+        <v>29400</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21">
+        <v>14120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>8340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23">
+        <v>7220</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>16630</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{352A72E2-4D67-F643-BFA7-A14AD7FC0F84}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Now setting factor levels.
</commit_message>
<xml_diff>
--- a/chapters/ch09-Agriculture/datasets/Ag Sankey.xlsx
+++ b/chapters/ch09-Agriculture/datasets/Ag Sankey.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E393FB39-D793-BC4A-9FDD-05C5AFFC9D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE01D29A-3162-4F40-9D7E-A911D19020AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="18820" xr2:uid="{AC192F2F-F1F4-CC41-936B-E23658F68C4F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
   <si>
     <t>x</t>
   </si>
@@ -146,10 +146,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,10 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCFF141-0596-C145-89EB-7AFC488BD6D2}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -841,11 +850,64 @@
         <v>34</v>
       </c>
       <c r="D16" t="s">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>68080</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="2">
-        <f>SUM(E9:E15)</f>
-        <v>1074590</v>
+      <c r="E17" s="4">
+        <f>SUM(E9:E15)-E16</f>
+        <v>1006510</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
+        <f>E16</f>
+        <v>68080</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="B19">
+        <v>5</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <f>E18</f>
+        <v>68080</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on D3 Sankey
</commit_message>
<xml_diff>
--- a/chapters/ch09-Agriculture/datasets/Ag Sankey.xlsx
+++ b/chapters/ch09-Agriculture/datasets/Ag Sankey.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matt/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE01D29A-3162-4F40-9D7E-A911D19020AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6083DB58-D19F-C04D-BB60-02F91617E5F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="820" windowWidth="28040" windowHeight="18820" xr2:uid="{AC192F2F-F1F4-CC41-936B-E23658F68C4F}"/>
+    <workbookView xWindow="20800" yWindow="500" windowWidth="28040" windowHeight="18820" activeTab="2" xr2:uid="{AC192F2F-F1F4-CC41-936B-E23658F68C4F}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="data to plot d3 nodes" sheetId="3" r:id="rId3"/>
+    <sheet name="data to plot d3 links" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="41">
   <si>
     <t>x</t>
   </si>
@@ -140,6 +142,24 @@
   </si>
   <si>
     <t>Available crops</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>node_id</t>
+  </si>
+  <si>
+    <t>node_group</t>
+  </si>
+  <si>
+    <t>source_char</t>
+  </si>
+  <si>
+    <t>target_char</t>
+  </si>
+  <si>
+    <t>link_group</t>
   </si>
 </sst>
 </file>
@@ -194,12 +214,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -254,6 +275,104 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6591299" y="2222388"/>
+          <a:ext cx="9335829" cy="7277212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>177799</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>190388</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>433128</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A39F096-17FE-A04F-B66B-7EE49F22FA59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6591299" y="2222388"/>
+          <a:ext cx="9335829" cy="7277212"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>406399</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>88788</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>661728</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{51CC319E-502F-A047-B135-0932AA2EBA80}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4343399" y="495188"/>
           <a:ext cx="9335829" cy="7277212"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -565,7 +684,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACCFF141-0596-C145-89EB-7AFC488BD6D2}">
   <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -1509,4 +1628,418 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3628D5E0-0D72-E747-A029-7862529EF0AD}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF42F68E-15E3-BC44-AFD6-17D948BAA47B}">
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4">
+        <v>153000</v>
+      </c>
+      <c r="D2" s="4" t="str">
+        <f>A2</f>
+        <v>Storage</v>
+      </c>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4">
+        <v>21290</v>
+      </c>
+      <c r="D3" s="4" t="str">
+        <f t="shared" ref="D3:D4" si="0">A3</f>
+        <v>Cultivated fields</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
+        <v>37920</v>
+      </c>
+      <c r="D4" s="4" t="str">
+        <f t="shared" si="0"/>
+        <v>Cultivated fields</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>